<commit_message>
Update 170723b: Worked on the BDA implementations
</commit_message>
<xml_diff>
--- a/www/MP4/COD_summary.xlsx
+++ b/www/MP4/COD_summary.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -502,19 +502,19 @@
         <v>34</v>
       </c>
       <c r="I2">
-        <v>1183.429267163598</v>
+        <v>1775.143900745396</v>
       </c>
       <c r="J2">
-        <v>2.366887774893887</v>
+        <v>13.37126326159791</v>
       </c>
       <c r="K2">
-        <v>0.5939999999999999</v>
+        <v>1.08</v>
       </c>
       <c r="L2">
-        <v>0.54</v>
+        <v>3.51</v>
       </c>
       <c r="M2">
-        <v>1.134</v>
+        <v>0.108</v>
       </c>
       <c r="N2">
         <v>108</v>
@@ -523,27 +523,702 @@
         <v>54</v>
       </c>
       <c r="P2">
-        <v>0.0001</v>
+        <v>0.00015</v>
       </c>
       <c r="Q2">
-        <v>0.0055</v>
+        <v>0.03</v>
       </c>
       <c r="R2">
-        <v>0.0055</v>
+        <v>0.01</v>
       </c>
       <c r="S2">
-        <v>0.01</v>
+        <v>0.065</v>
       </c>
       <c r="T2">
-        <v>0.021</v>
+        <v>0.002</v>
       </c>
       <c r="U2">
         <v>1</v>
       </c>
       <c r="V2">
+        <v>15</v>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>SVEIRD</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2018-08-02</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>11834489</v>
+      </c>
+      <c r="C3">
+        <v>11832504</v>
+      </c>
+      <c r="D3">
+        <v>1775</v>
+      </c>
+      <c r="E3">
+        <v>120</v>
+      </c>
+      <c r="F3">
+        <v>51</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>34</v>
+      </c>
+      <c r="I3">
+        <v>1774.875623470791</v>
+      </c>
+      <c r="J3">
+        <v>12.73975204753981</v>
+      </c>
+      <c r="K3">
+        <v>1.158469110011569</v>
+      </c>
+      <c r="L3">
+        <v>2.23002</v>
+      </c>
+      <c r="M3">
+        <v>0.068616</v>
+      </c>
+      <c r="N3">
+        <v>121.371263261598</v>
+      </c>
+      <c r="O3">
+        <v>55.08000000000004</v>
+      </c>
+      <c r="P3">
+        <v>0.00015</v>
+      </c>
+      <c r="Q3">
+        <v>0.03</v>
+      </c>
+      <c r="R3">
+        <v>0.01</v>
+      </c>
+      <c r="S3">
+        <v>0.065</v>
+      </c>
+      <c r="T3">
+        <v>0.002</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>15</v>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>SVEIRD</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2018-08-03</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>11834489</v>
+      </c>
+      <c r="C4">
+        <v>11830717</v>
+      </c>
+      <c r="D4">
+        <v>3550</v>
+      </c>
+      <c r="E4">
+        <v>132</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>34</v>
+      </c>
+      <c r="I4">
+        <v>1774.607481164467</v>
+      </c>
+      <c r="J4">
+        <v>12.44674784837062</v>
+      </c>
+      <c r="K4">
+        <v>1.231936614936079</v>
+      </c>
+      <c r="L4">
+        <v>2.130950231618221</v>
+      </c>
+      <c r="M4">
+        <v>0.06556769943440682</v>
+      </c>
+      <c r="N4">
+        <v>134.1110153091378</v>
+      </c>
+      <c r="O4">
+        <v>56.23846911001161</v>
+      </c>
+      <c r="P4">
+        <v>0.00015</v>
+      </c>
+      <c r="Q4">
+        <v>0.03</v>
+      </c>
+      <c r="R4">
+        <v>0.01</v>
+      </c>
+      <c r="S4">
+        <v>0.065</v>
+      </c>
+      <c r="T4">
+        <v>0.002</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>15</v>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>SVEIRD</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2018-08-04</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>11834489</v>
+      </c>
+      <c r="C5">
+        <v>11828929</v>
+      </c>
+      <c r="D5">
+        <v>5325</v>
+      </c>
+      <c r="E5">
+        <v>143</v>
+      </c>
+      <c r="F5">
+        <v>49</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>34</v>
+      </c>
+      <c r="I5">
+        <v>1774.339423030118</v>
+      </c>
+      <c r="J5">
+        <v>12.19782946668761</v>
+      </c>
+      <c r="K5">
+        <v>1.302636971036312</v>
+      </c>
+      <c r="L5">
+        <v>2.041834782010154</v>
+      </c>
+      <c r="M5">
+        <v>0.06282568560031242</v>
+      </c>
+      <c r="N5">
+        <v>146.5577631575085</v>
+      </c>
+      <c r="O5">
+        <v>57.47040572494771</v>
+      </c>
+      <c r="P5">
+        <v>0.00015</v>
+      </c>
+      <c r="Q5">
+        <v>0.03</v>
+      </c>
+      <c r="R5">
+        <v>0.01</v>
+      </c>
+      <c r="S5">
+        <v>0.065</v>
+      </c>
+      <c r="T5">
+        <v>0.002</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>15</v>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>SVEIRD</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2018-08-05</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>11834489</v>
+      </c>
+      <c r="C6">
+        <v>11827143</v>
+      </c>
+      <c r="D6">
+        <v>7099</v>
+      </c>
+      <c r="E6">
+        <v>154</v>
+      </c>
+      <c r="F6">
+        <v>49</v>
+      </c>
+      <c r="G6">
         <v>10</v>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="H6">
+        <v>34</v>
+      </c>
+      <c r="I6">
+        <v>1774.071442442239</v>
+      </c>
+      <c r="J6">
+        <v>11.98968540732331</v>
+      </c>
+      <c r="K6">
+        <v>1.381307462295751</v>
+      </c>
+      <c r="L6">
+        <v>3.156089839325856</v>
+      </c>
+      <c r="M6">
+        <v>0.09711045659464172</v>
+      </c>
+      <c r="N6">
+        <v>158.7555926241962</v>
+      </c>
+      <c r="O6">
+        <v>58.77304269598401</v>
+      </c>
+      <c r="P6">
+        <v>0.00015</v>
+      </c>
+      <c r="Q6">
+        <v>0.03</v>
+      </c>
+      <c r="R6">
+        <v>0.01</v>
+      </c>
+      <c r="S6">
+        <v>0.065</v>
+      </c>
+      <c r="T6">
+        <v>0.002</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>15</v>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>SVEIRD</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2018-08-06</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>11834489</v>
+      </c>
+      <c r="C7">
+        <v>11825357</v>
+      </c>
+      <c r="D7">
+        <v>8873</v>
+      </c>
+      <c r="E7">
+        <v>165</v>
+      </c>
+      <c r="F7">
+        <v>47</v>
+      </c>
+      <c r="G7">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>34</v>
+      </c>
+      <c r="I7">
+        <v>1773.803533273062</v>
+      </c>
+      <c r="J7">
+        <v>11.43811355674682</v>
+      </c>
+      <c r="K7">
+        <v>1.500991779390872</v>
+      </c>
+      <c r="L7">
+        <v>1.89006333239834</v>
+      </c>
+      <c r="M7">
+        <v>0.05815579484302584</v>
+      </c>
+      <c r="N7">
+        <v>170.7452780315195</v>
+      </c>
+      <c r="O7">
+        <v>60.15435015827978</v>
+      </c>
+      <c r="P7">
+        <v>0.00015</v>
+      </c>
+      <c r="Q7">
+        <v>0.03</v>
+      </c>
+      <c r="R7">
+        <v>0.01</v>
+      </c>
+      <c r="S7">
+        <v>0.065</v>
+      </c>
+      <c r="T7">
+        <v>0.002</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>15</v>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>SVEIRD</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2018-08-07</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>11834489</v>
+      </c>
+      <c r="C8">
+        <v>11823572</v>
+      </c>
+      <c r="D8">
+        <v>10647</v>
+      </c>
+      <c r="E8">
+        <v>175</v>
+      </c>
+      <c r="F8">
+        <v>46</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>34</v>
+      </c>
+      <c r="I8">
+        <v>1773.535747026039</v>
+      </c>
+      <c r="J8">
+        <v>11.31960157512937</v>
+      </c>
+      <c r="K8">
+        <v>1.57421911608137</v>
+      </c>
+      <c r="L8">
+        <v>2.481408093863778</v>
+      </c>
+      <c r="M8">
+        <v>0.07635101827273164</v>
+      </c>
+      <c r="N8">
+        <v>182.1833915882663</v>
+      </c>
+      <c r="O8">
+        <v>61.65534193767067</v>
+      </c>
+      <c r="P8">
+        <v>0.00015</v>
+      </c>
+      <c r="Q8">
+        <v>0.03</v>
+      </c>
+      <c r="R8">
+        <v>0.01</v>
+      </c>
+      <c r="S8">
+        <v>0.065</v>
+      </c>
+      <c r="T8">
+        <v>0.002</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>15</v>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>SVEIRD</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2018-08-08</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>11834489</v>
+      </c>
+      <c r="C9">
+        <v>11821787</v>
+      </c>
+      <c r="D9">
+        <v>12420</v>
+      </c>
+      <c r="E9">
+        <v>184</v>
+      </c>
+      <c r="F9">
+        <v>45</v>
+      </c>
+      <c r="G9">
+        <v>17</v>
+      </c>
+      <c r="H9">
+        <v>35</v>
+      </c>
+      <c r="I9">
+        <v>1773.268018723749</v>
+      </c>
+      <c r="J9">
+        <v>11.06567226716502</v>
+      </c>
+      <c r="K9">
+        <v>1.656545192275124</v>
+      </c>
+      <c r="L9">
+        <v>2.171655481216805</v>
+      </c>
+      <c r="M9">
+        <v>0.06682016865282477</v>
+      </c>
+      <c r="N9">
+        <v>193.5029931633956</v>
+      </c>
+      <c r="O9">
+        <v>63.22956105375204</v>
+      </c>
+      <c r="P9">
+        <v>0.00015</v>
+      </c>
+      <c r="Q9">
+        <v>0.03</v>
+      </c>
+      <c r="R9">
+        <v>0.01</v>
+      </c>
+      <c r="S9">
+        <v>0.065</v>
+      </c>
+      <c r="T9">
+        <v>0.002</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>15</v>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>SVEIRD</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2018-08-09</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>11834489</v>
+      </c>
+      <c r="C10">
+        <v>11820002</v>
+      </c>
+      <c r="D10">
+        <v>14194</v>
+      </c>
+      <c r="E10">
+        <v>194</v>
+      </c>
+      <c r="F10">
+        <v>45</v>
+      </c>
+      <c r="G10">
+        <v>20</v>
+      </c>
+      <c r="H10">
+        <v>35</v>
+      </c>
+      <c r="I10">
+        <v>1773.0003686701</v>
+      </c>
+      <c r="J10">
+        <v>10.920877402829</v>
+      </c>
+      <c r="K10">
+        <v>1.756893851467628</v>
+      </c>
+      <c r="L10">
+        <v>1.604509668604567</v>
+      </c>
+      <c r="M10">
+        <v>0.04936952826475591</v>
+      </c>
+      <c r="N10">
+        <v>204.5686654305606</v>
+      </c>
+      <c r="O10">
+        <v>64.8861062460272</v>
+      </c>
+      <c r="P10">
+        <v>0.00015</v>
+      </c>
+      <c r="Q10">
+        <v>0.03</v>
+      </c>
+      <c r="R10">
+        <v>0.01</v>
+      </c>
+      <c r="S10">
+        <v>0.065</v>
+      </c>
+      <c r="T10">
+        <v>0.002</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>15</v>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>SVEIRD</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2018-08-10</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>11834489</v>
+      </c>
+      <c r="C11">
+        <v>11818219</v>
+      </c>
+      <c r="D11">
+        <v>15967</v>
+      </c>
+      <c r="E11">
+        <v>203</v>
+      </c>
+      <c r="F11">
+        <v>45</v>
+      </c>
+      <c r="G11">
+        <v>21</v>
+      </c>
+      <c r="H11">
+        <v>35</v>
+      </c>
+      <c r="I11">
+        <v>1772.732780483186</v>
+      </c>
+      <c r="J11">
+        <v>10.96418237684003</v>
+      </c>
+      <c r="K11">
+        <v>1.838263936851671</v>
+      </c>
+      <c r="L11">
+        <v>2.43490979030852</v>
+      </c>
+      <c r="M11">
+        <v>0.07492030124026215</v>
+      </c>
+      <c r="N11">
+        <v>215.4895428333898</v>
+      </c>
+      <c r="O11">
+        <v>66.64300009749478</v>
+      </c>
+      <c r="P11">
+        <v>0.00015</v>
+      </c>
+      <c r="Q11">
+        <v>0.03</v>
+      </c>
+      <c r="R11">
+        <v>0.01</v>
+      </c>
+      <c r="S11">
+        <v>0.065</v>
+      </c>
+      <c r="T11">
+        <v>0.002</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>15</v>
+      </c>
+      <c r="W11" t="inlineStr">
         <is>
           <t>SVEIRD</t>
         </is>

</xml_diff>

<commit_message>
minor code changes by AK
</commit_message>
<xml_diff>
--- a/www/MP4/COD_summary.xlsx
+++ b/www/MP4/COD_summary.xlsx
@@ -505,7 +505,7 @@
         <v>1775.143900745396</v>
       </c>
       <c r="J2">
-        <v>13.37126326159791</v>
+        <v>13.3808623608729</v>
       </c>
       <c r="K2">
         <v>1.08</v>
@@ -577,13 +577,13 @@
         <v>34</v>
       </c>
       <c r="I3">
-        <v>1774.875623470791</v>
+        <v>1774.875622030926</v>
       </c>
       <c r="J3">
-        <v>12.73975204753981</v>
+        <v>12.74777477556336</v>
       </c>
       <c r="K3">
-        <v>1.158469110011569</v>
+        <v>1.159414701257576</v>
       </c>
       <c r="L3">
         <v>2.23002</v>
@@ -592,7 +592,7 @@
         <v>0.068616</v>
       </c>
       <c r="N3">
-        <v>121.371263261598</v>
+        <v>121.380862360873</v>
       </c>
       <c r="O3">
         <v>55.08000000000004</v>
@@ -652,25 +652,25 @@
         <v>34</v>
       </c>
       <c r="I4">
-        <v>1774.607481164467</v>
+        <v>1774.607478521407</v>
       </c>
       <c r="J4">
-        <v>12.44674784837062</v>
+        <v>12.45488223305614</v>
       </c>
       <c r="K4">
-        <v>1.231936614936079</v>
+        <v>1.233763307075057</v>
       </c>
       <c r="L4">
-        <v>2.130950231618221</v>
+        <v>2.131015916978649</v>
       </c>
       <c r="M4">
-        <v>0.06556769943440682</v>
+        <v>0.06556972052241997</v>
       </c>
       <c r="N4">
-        <v>134.1110153091378</v>
+        <v>134.1286371364363</v>
       </c>
       <c r="O4">
-        <v>56.23846911001161</v>
+        <v>56.23941470125762</v>
       </c>
       <c r="P4">
         <v>0.00015</v>
@@ -727,25 +727,25 @@
         <v>34</v>
       </c>
       <c r="I5">
-        <v>1774.339423030118</v>
+        <v>1774.3394191673</v>
       </c>
       <c r="J5">
-        <v>12.19782946668761</v>
+        <v>12.20629766163735</v>
       </c>
       <c r="K5">
-        <v>1.302636971036312</v>
+        <v>1.30528449468716</v>
       </c>
       <c r="L5">
-        <v>2.041834782010154</v>
+        <v>2.042023219613001</v>
       </c>
       <c r="M5">
-        <v>0.06282568560031242</v>
+        <v>0.06283148368040004</v>
       </c>
       <c r="N5">
-        <v>146.5577631575085</v>
+        <v>146.5835193694924</v>
       </c>
       <c r="O5">
-        <v>57.47040572494771</v>
+        <v>57.47317800833267</v>
       </c>
       <c r="P5">
         <v>0.00015</v>
@@ -802,25 +802,25 @@
         <v>34</v>
       </c>
       <c r="I6">
-        <v>1774.071442442239</v>
+        <v>1774.071437309771</v>
       </c>
       <c r="J6">
-        <v>11.98968540732331</v>
+        <v>11.99866664560645</v>
       </c>
       <c r="K6">
-        <v>1.381307462295751</v>
+        <v>1.374320712981774</v>
       </c>
       <c r="L6">
-        <v>3.156089839325856</v>
+        <v>3.156425100544646</v>
       </c>
       <c r="M6">
-        <v>0.09711045659464172</v>
+        <v>0.09712077232445063</v>
       </c>
       <c r="N6">
-        <v>158.7555926241962</v>
+        <v>158.7898170311298</v>
       </c>
       <c r="O6">
-        <v>58.77304269598401</v>
+        <v>58.77846250301983</v>
       </c>
       <c r="P6">
         <v>0.00015</v>
@@ -877,25 +877,25 @@
         <v>34</v>
       </c>
       <c r="I7">
-        <v>1773.803533273062</v>
+        <v>1773.803526794177</v>
       </c>
       <c r="J7">
-        <v>11.43811355674682</v>
+        <v>11.47324891637379</v>
       </c>
       <c r="K7">
-        <v>1.500991779390872</v>
+        <v>1.494693836948371</v>
       </c>
       <c r="L7">
-        <v>1.89006333239834</v>
+        <v>1.890639607614224</v>
       </c>
       <c r="M7">
-        <v>0.05815579484302584</v>
+        <v>0.05817352638812998</v>
       </c>
       <c r="N7">
-        <v>170.7452780315195</v>
+        <v>170.7884836767364</v>
       </c>
       <c r="O7">
-        <v>60.15435015827978</v>
+        <v>60.1527832160016</v>
       </c>
       <c r="P7">
         <v>0.00015</v>
@@ -952,25 +952,25 @@
         <v>34</v>
       </c>
       <c r="I8">
-        <v>1773.535747026039</v>
+        <v>1773.535735277823</v>
       </c>
       <c r="J8">
-        <v>11.31960157512937</v>
+        <v>11.35245243162619</v>
       </c>
       <c r="K8">
-        <v>1.57421911608137</v>
+        <v>1.566858109687555</v>
       </c>
       <c r="L8">
-        <v>2.481408093863778</v>
+        <v>2.482194601935355</v>
       </c>
       <c r="M8">
-        <v>0.07635101827273164</v>
+        <v>0.07637521852108783</v>
       </c>
       <c r="N8">
-        <v>182.1833915882663</v>
+        <v>182.2617325931104</v>
       </c>
       <c r="O8">
-        <v>61.65534193767067</v>
+        <v>61.64747705294996</v>
       </c>
       <c r="P8">
         <v>0.00015</v>
@@ -1027,25 +1027,25 @@
         <v>35</v>
       </c>
       <c r="I9">
-        <v>1773.268018723749</v>
+        <v>1773.268002049666</v>
       </c>
       <c r="J9">
-        <v>11.06567226716502</v>
+        <v>11.09650387758536</v>
       </c>
       <c r="K9">
-        <v>1.656545192275124</v>
+        <v>1.659139473800495</v>
       </c>
       <c r="L9">
-        <v>2.171655481216805</v>
+        <v>2.172733351266169</v>
       </c>
       <c r="M9">
-        <v>0.06682016865282477</v>
+        <v>0.0668533338851129</v>
       </c>
       <c r="N9">
-        <v>193.5029931633956</v>
+        <v>193.6141850247366</v>
       </c>
       <c r="O9">
-        <v>63.22956105375204</v>
+        <v>63.2143351626375</v>
       </c>
       <c r="P9">
         <v>0.00015</v>
@@ -1102,25 +1102,25 @@
         <v>35</v>
       </c>
       <c r="I10">
-        <v>1773.0003686701</v>
+        <v>1773.000347373775</v>
       </c>
       <c r="J10">
-        <v>10.920877402829</v>
+        <v>10.94959980496654</v>
       </c>
       <c r="K10">
-        <v>1.756893851467628</v>
+        <v>1.780116714042583</v>
       </c>
       <c r="L10">
-        <v>1.604509668604567</v>
+        <v>1.540244479045344</v>
       </c>
       <c r="M10">
-        <v>0.04936952826475591</v>
+        <v>0.04739213781677981</v>
       </c>
       <c r="N10">
-        <v>204.5686654305606</v>
+        <v>204.7106889023218</v>
       </c>
       <c r="O10">
-        <v>64.8861062460272</v>
+        <v>64.87347463643796</v>
       </c>
       <c r="P10">
         <v>0.00015</v>
@@ -1159,7 +1159,7 @@
         <v>11834489</v>
       </c>
       <c r="C11">
-        <v>11818219</v>
+        <v>11818218</v>
       </c>
       <c r="D11">
         <v>15967</v>
@@ -1177,25 +1177,25 @@
         <v>35</v>
       </c>
       <c r="I11">
-        <v>1772.732780483186</v>
+        <v>1772.732754881697</v>
       </c>
       <c r="J11">
-        <v>10.96418237684003</v>
+        <v>10.98443980637041</v>
       </c>
       <c r="K11">
-        <v>1.838263936851671</v>
+        <v>1.853240598998291</v>
       </c>
       <c r="L11">
-        <v>2.43490979030852</v>
+        <v>2.569908419474952</v>
       </c>
       <c r="M11">
-        <v>0.07492030124026215</v>
+        <v>0.0790741052146139</v>
       </c>
       <c r="N11">
-        <v>215.4895428333898</v>
+        <v>215.6602887072884</v>
       </c>
       <c r="O11">
-        <v>66.64300009749478</v>
+        <v>66.65359135048054</v>
       </c>
       <c r="P11">
         <v>0.00015</v>

</xml_diff>